<commit_message>
Adicionar páginas para gerenciamento de turmas e professores, incluindo funcionalidades para adicionar, listar e atribuir disciplinas.
</commit_message>
<xml_diff>
--- a/solver_teachers/alocacao_turmas.xlsx
+++ b/solver_teachers/alocacao_turmas.xlsx
@@ -473,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Thiago (Ciências)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Pedro (Português)</t>
         </is>
       </c>
     </row>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Camila (Artes)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Pedro (Português)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
     </row>
@@ -537,27 +537,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -579,17 +579,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Thiago (Ciências)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
     </row>
@@ -601,27 +601,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Pedro (Português)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Pedro (Português)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Horsão (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lucas (Matemática)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
     </row>
@@ -679,27 +679,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
     </row>
@@ -711,27 +711,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Alan (Matemática)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Camila (Artes)</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alan (Português)</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
     </row>
@@ -743,27 +743,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Pedro (Português)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
     </row>
@@ -775,27 +775,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Bignicius (Ciências)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bignicius (Ciências)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Pedro (Português)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pedro (Português)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Camila (Artes)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alan (Português)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Alan (Português)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bignicius (Ciências)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Straw (Matemática)</t>
         </is>
       </c>
     </row>
@@ -807,27 +807,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Pedro (Português)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bignicius (Ciências)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
     </row>
@@ -885,27 +885,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Straw (Artes)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
     </row>
@@ -917,27 +917,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Straw (Artes)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
     </row>
@@ -949,27 +949,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Camila (Artes)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Alan (Português)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Bignicius (Ciências)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Jorge (Português)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jorge (Português)</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
     </row>
@@ -981,27 +981,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Camila (Artes)</t>
         </is>
       </c>
     </row>
@@ -1013,27 +1013,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Straw (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bignicius (Ciências)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Straw (Artes)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
     </row>
@@ -1091,27 +1091,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1133,17 +1133,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
     </row>
@@ -1155,27 +1155,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Jorge (Geografia)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alan (Português)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Alan (Matemática)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Alan (Matemática)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Camila (Artes)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Rogério (Matemática)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Rogério (Matemática)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Alan (Português)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Alan (Português)</t>
         </is>
       </c>
     </row>
@@ -1187,22 +1187,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Bignicius (Ciências)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Camila (Artes)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1224,22 +1224,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Alan (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Rogério (Matemática)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
     </row>
@@ -1297,27 +1297,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Thiago (Ciências)</t>
         </is>
       </c>
     </row>
@@ -1329,27 +1329,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Camila (Artes)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Thiago (Ciências)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
     </row>
@@ -1361,27 +1361,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Camila (Artes)</t>
+          <t>Carlos (Educação Física)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bignicius (Ciências)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
     </row>
@@ -1393,27 +1393,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bignicius (Ciências)</t>
+          <t>Thiago (Ciências)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Alan (Matemática)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Camila (Artes)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Thiago (Ciências)</t>
         </is>
       </c>
     </row>
@@ -1425,27 +1425,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Pedro (História)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Beatriz (Inglês)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Alan (Português)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Jorge (Português)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Thiago (Matemática)</t>
+          <t>Jorge (Geografia)</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1476,85 +1476,187 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Horsão</t>
+          <t>Bignicius</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Bignicius</t>
+          <t>Jorge</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Jorge</t>
+          <t>Camila</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Rogério</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Straw</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Camila</t>
+          <t>Beatriz</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Thiago</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Renata</t>
+          <t>Ocupação</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Ocupação</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+          <t>Alan</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bignicius</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Jorge</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Camila</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Thiago</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Beatriz</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
         <v>20</v>
-      </c>
-      <c r="C2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>23</v>
-      </c>
-      <c r="H2" t="n">
-        <v>10</v>
-      </c>
-      <c r="I2" t="n">
-        <v>12</v>
-      </c>
-      <c r="J2" t="n">
-        <v>12</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>